<commit_message>
Add images and latex report
</commit_message>
<xml_diff>
--- a/ModelFitting/data_fitting.xlsx
+++ b/ModelFitting/data_fitting.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24F923C-5DED-400C-BC44-E8FF93C6D850}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1896EC1D-97A9-4089-8481-2355E71D2087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raindrops" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>v_term</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Estimate</t>
+  </si>
+  <si>
+    <t>Residuals</t>
   </si>
 </sst>
 </file>
@@ -1530,6 +1533,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Stress (lb/inch^2)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.43729746281714788"/>
+              <c:y val="0.90645815106445027"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1592,6 +1658,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Elongation (10^(-5)inch/inch)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2149,11 +2270,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Wire Stress'!$C$1</c:f>
+              <c:f>'Wire Stress'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Estimation</c:v>
+                  <c:v>Residuals</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2180,70 +2301,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.23618941382327205"/>
-                  <c:y val="5.513888888888889E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Wire Stress'!$A$2:$A$12</c:f>
@@ -2288,42 +2345,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Wire Stress'!$C$2:$C$12</c:f>
+              <c:f>'Wire Stress'!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-5.3999999999999986</c:v>
+                  <c:v>5.0499999999999972</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.600000000000001</c:v>
+                  <c:v>3.6999999999999957</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54.6</c:v>
+                  <c:v>0.99999999999999289</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>94.6</c:v>
+                  <c:v>-2.7000000000000171</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>134.6</c:v>
+                  <c:v>-3.4000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>174.6</c:v>
+                  <c:v>-5.0999999999999943</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>214.6</c:v>
+                  <c:v>-2.8000000000000114</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>254.6</c:v>
+                  <c:v>-3.5000000000000568</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>294.60000000000002</c:v>
+                  <c:v>-3.2000000000000455</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>334.6</c:v>
+                  <c:v>2.0999999999999659</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>374.6</c:v>
+                  <c:v>8.3999999999999773</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2331,7 +2388,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BCCA-4F53-9F0B-EF9BC5C68D97}"/>
+              <c16:uniqueId val="{00000000-D7E4-41C9-9C28-18C08C77FAC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2343,11 +2400,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="492869880"/>
-        <c:axId val="492868920"/>
+        <c:axId val="403243448"/>
+        <c:axId val="403243768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="492869880"/>
+        <c:axId val="403243448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2367,6 +2424,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Stress (lb/in^s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2404,12 +2516,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492868920"/>
+        <c:crossAx val="403243768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="492868920"/>
+        <c:axId val="403243768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2429,6 +2541,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Residuals</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2466,7 +2633,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492869880"/>
+        <c:crossAx val="403243448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2799,6 +2966,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Diameter</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2861,6 +3083,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Volume</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3009,11 +3286,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Pines!$C$1</c:f>
+              <c:f>Pines!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Estimate</c:v>
+                  <c:v>Residuals</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3040,182 +3317,110 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Pines!$B$2:$B$16</c:f>
+              <c:f>Pines!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>113</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>141</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>123</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>187</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>192</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>205</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>252</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>259</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>294</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Pines!$C$2:$C$16</c:f>
+              <c:f>Pines!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>20.870921979927346</c:v>
+                  <c:v>-1.8709219799273455</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.46362248303701</c:v>
+                  <c:v>-4.4636224830370104</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.54164090044322</c:v>
+                  <c:v>-2.5416409004432197</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.415206704205637</c:v>
+                  <c:v>4.5847932957943627</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53.272891535453795</c:v>
+                  <c:v>3.7271084645462054</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>68.986483073060654</c:v>
+                  <c:v>2.0135169269393458</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>98.025682666933292</c:v>
+                  <c:v>14.974317333066708</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>134.39132296431976</c:v>
+                  <c:v>6.6086770356802447</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>148.29104003789314</c:v>
+                  <c:v>-25.29104003789314</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>163.13351425305916</c:v>
+                  <c:v>23.866485746940839</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>213.64253903374967</c:v>
+                  <c:v>-21.642539033749671</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>232.58158344625292</c:v>
+                  <c:v>-27.581583446252921</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>252.62662950005435</c:v>
+                  <c:v>-0.62662950005434936</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>273.8106020071458</c:v>
+                  <c:v>-14.810602007145803</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>319.7274575077202</c:v>
+                  <c:v>-25.727457507720203</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3223,7 +3428,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-95EE-4326-9691-BD80FF314325}"/>
+              <c16:uniqueId val="{00000000-702B-4501-9417-783840CF3204}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3235,11 +3440,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="419874736"/>
-        <c:axId val="487983664"/>
+        <c:axId val="241104560"/>
+        <c:axId val="245828792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="419874736"/>
+        <c:axId val="241104560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3296,12 +3501,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487983664"/>
+        <c:crossAx val="245828792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="487983664"/>
+        <c:axId val="245828792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3358,7 +3563,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419874736"/>
+        <c:crossAx val="241104560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3871,11 +4076,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planets!$D$1</c:f>
+              <c:f>Planets!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Estimate</c:v>
+                  <c:v>Residuals</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3902,50 +4107,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Planets!$B$2:$B$10</c:f>
@@ -3984,36 +4145,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Planets!$D$2:$D$10</c:f>
+              <c:f>Planets!$E$2:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>59.353049318984404</c:v>
+                  <c:v>1.4530493189844051</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110.97954334487116</c:v>
+                  <c:v>2.7795433448711577</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>153.2203668041796</c:v>
+                  <c:v>3.6203668041796107</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>233.57467115870674</c:v>
+                  <c:v>5.6746711587067296</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>796.85562975752998</c:v>
+                  <c:v>18.75562975752996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1461.5298349424061</c:v>
+                  <c:v>33.329834942406023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2938.7954248969354</c:v>
+                  <c:v>100.89542489693531</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4605.5164992718474</c:v>
+                  <c:v>116.61649927184772</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6054.760911587291</c:v>
+                  <c:v>178.06091158729123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4021,7 +4182,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CD88-4EB1-BDD4-3E1A6E4DDAD7}"/>
+              <c16:uniqueId val="{00000000-4906-4726-9534-331953E88400}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4033,11 +4194,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="468213816"/>
-        <c:axId val="468215416"/>
+        <c:axId val="245815280"/>
+        <c:axId val="241099120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="468213816"/>
+        <c:axId val="245815280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4094,12 +4255,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="468215416"/>
+        <c:crossAx val="241099120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="468215416"/>
+        <c:axId val="241099120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4156,7 +4317,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="468213816"/>
+        <c:crossAx val="245815280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9297,16 +9458,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>311942</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>111919</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>450055</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2382</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>350042</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>140494</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>488155</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>30957</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9370,22 +9531,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>335755</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>150018</xdr:rowOff>
+      <xdr:colOff>626267</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>26193</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>373855</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>178593</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>16667</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>54768</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EAE4396-DD33-4A82-A258-50A86268FF33}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6259C2E3-18E4-45F6-88EA-B75FCCFAB0BF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9447,22 +9608,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>335756</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>16669</xdr:rowOff>
+      <xdr:colOff>397668</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>30956</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>373856</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>45244</xdr:rowOff>
+      <xdr:colOff>435768</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FF69019-F3B3-4B3A-91DE-BD7B99B5B4C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB5A2852-630B-4B6E-9E7F-DB91CC23B627}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9524,22 +9685,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>597694</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>116681</xdr:rowOff>
+      <xdr:colOff>883443</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>88106</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>411956</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>145256</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>50005</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>116681</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6971CE1C-52C9-473F-BE9A-01A843B4A8F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C0D4F67-C041-4B30-B870-9A7DB317F018}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9825,7 +9986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
@@ -10502,10 +10663,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10514,7 +10675,7 @@
     <col min="2" max="2" width="26.86328125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -10524,8 +10685,11 @@
       <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>5</v>
       </c>
@@ -10533,11 +10697,15 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f>4*A2-25.4</f>
-        <v>-5.3999999999999986</v>
+        <f>4.07*A2-25.4</f>
+        <v>-5.0499999999999972</v>
+      </c>
+      <c r="D2">
+        <f>B2 - C2</f>
+        <v>5.0499999999999972</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -10545,11 +10713,15 @@
         <v>19</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C12" si="0">4*A3-25.4</f>
-        <v>14.600000000000001</v>
+        <f t="shared" ref="C3:C12" si="0">4.07*A3-25.4</f>
+        <v>15.300000000000004</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D11" si="1">B3 - C3</f>
+        <v>3.6999999999999957</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>20</v>
       </c>
@@ -10558,10 +10730,14 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>54.6</v>
+        <v>56.000000000000007</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>0.99999999999999289</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>30</v>
       </c>
@@ -10570,10 +10746,14 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>94.6</v>
+        <v>96.700000000000017</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>-2.7000000000000171</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>40</v>
       </c>
@@ -10582,10 +10762,14 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>134.6</v>
+        <v>137.4</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>-3.4000000000000057</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>50</v>
       </c>
@@ -10594,10 +10778,14 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>174.6</v>
+        <v>178.1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>-5.0999999999999943</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>60</v>
       </c>
@@ -10606,10 +10794,14 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>214.6</v>
+        <v>218.8</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>-2.8000000000000114</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>70</v>
       </c>
@@ -10618,10 +10810,14 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>254.6</v>
+        <v>259.50000000000006</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>-3.5000000000000568</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>80</v>
       </c>
@@ -10630,10 +10826,14 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>294.60000000000002</v>
+        <v>300.20000000000005</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>-3.2000000000000455</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>90</v>
       </c>
@@ -10642,10 +10842,14 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>334.6</v>
+        <v>340.90000000000003</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2.0999999999999659</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>100</v>
       </c>
@@ -10654,7 +10858,11 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>374.6</v>
+        <v>381.6</v>
+      </c>
+      <c r="D12">
+        <f>B12 - C12</f>
+        <v>8.3999999999999773</v>
       </c>
     </row>
   </sheetData>
@@ -10666,10 +10874,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10678,7 +10886,7 @@
     <col min="2" max="2" width="20" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -10688,8 +10896,11 @@
       <c r="C1" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>17</v>
       </c>
@@ -10700,8 +10911,12 @@
         <f>0.0032*A2^3.1</f>
         <v>20.870921979927346</v>
       </c>
+      <c r="D2">
+        <f>B2-C2</f>
+        <v>-1.8709219799273455</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>19</v>
       </c>
@@ -10712,8 +10927,12 @@
         <f t="shared" ref="C3:C16" si="0">0.0032*A3^3.1</f>
         <v>29.46362248303701</v>
       </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D16" si="1">B3-C3</f>
+        <v>-4.4636224830370104</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>20</v>
       </c>
@@ -10724,8 +10943,12 @@
         <f t="shared" si="0"/>
         <v>34.54164090044322</v>
       </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>-2.5416409004432197</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>22</v>
       </c>
@@ -10736,8 +10959,12 @@
         <f t="shared" si="0"/>
         <v>46.415206704205637</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>4.5847932957943627</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>23</v>
       </c>
@@ -10748,8 +10975,12 @@
         <f t="shared" si="0"/>
         <v>53.272891535453795</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>3.7271084645462054</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>25</v>
       </c>
@@ -10760,8 +10991,12 @@
         <f t="shared" si="0"/>
         <v>68.986483073060654</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>2.0135169269393458</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>28</v>
       </c>
@@ -10772,8 +11007,12 @@
         <f t="shared" si="0"/>
         <v>98.025682666933292</v>
       </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>14.974317333066708</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>31</v>
       </c>
@@ -10784,8 +11023,12 @@
         <f t="shared" si="0"/>
         <v>134.39132296431976</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>6.6086770356802447</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>32</v>
       </c>
@@ -10796,8 +11039,12 @@
         <f t="shared" si="0"/>
         <v>148.29104003789314</v>
       </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>-25.29104003789314</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>33</v>
       </c>
@@ -10808,8 +11055,12 @@
         <f t="shared" si="0"/>
         <v>163.13351425305916</v>
       </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>23.866485746940839</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>36</v>
       </c>
@@ -10820,8 +11071,12 @@
         <f t="shared" si="0"/>
         <v>213.64253903374967</v>
       </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>-21.642539033749671</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>37</v>
       </c>
@@ -10832,8 +11087,12 @@
         <f t="shared" si="0"/>
         <v>232.58158344625292</v>
       </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>-27.581583446252921</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>38</v>
       </c>
@@ -10844,8 +11103,12 @@
         <f t="shared" si="0"/>
         <v>252.62662950005435</v>
       </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>-0.62662950005434936</v>
+      </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>39</v>
       </c>
@@ -10856,8 +11119,12 @@
         <f t="shared" si="0"/>
         <v>273.8106020071458</v>
       </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>-14.810602007145803</v>
+      </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>41</v>
       </c>
@@ -10867,6 +11134,10 @@
       <c r="C16">
         <f t="shared" si="0"/>
         <v>319.7274575077202</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>-25.727457507720203</v>
       </c>
     </row>
   </sheetData>
@@ -10878,10 +11149,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D1" activeCellId="1" sqref="B1:B10 D1:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" activeCellId="1" sqref="B1:B10 E1:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10891,7 +11162,7 @@
     <col min="3" max="3" width="39.3984375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -10904,8 +11175,11 @@
       <c r="D1" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -10919,8 +11193,12 @@
         <f>3*B2^(2/3)</f>
         <v>59.353049318984404</v>
       </c>
+      <c r="E2">
+        <f>D2-C2</f>
+        <v>1.4530493189844051</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -10934,8 +11212,12 @@
         <f t="shared" ref="D3:D10" si="0">3*B3^(2/3)</f>
         <v>110.97954334487116</v>
       </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="1">D3-C3</f>
+        <v>2.7795433448711577</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -10949,8 +11231,12 @@
         <f t="shared" si="0"/>
         <v>153.2203668041796</v>
       </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>3.6203668041796107</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -10964,8 +11250,12 @@
         <f t="shared" si="0"/>
         <v>233.57467115870674</v>
       </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>5.6746711587067296</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -10979,8 +11269,12 @@
         <f t="shared" si="0"/>
         <v>796.85562975752998</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>18.75562975752996</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -10994,8 +11288,12 @@
         <f t="shared" si="0"/>
         <v>1461.5298349424061</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>33.329834942406023</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -11009,8 +11307,12 @@
         <f t="shared" si="0"/>
         <v>2938.7954248969354</v>
       </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>100.89542489693531</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -11024,8 +11326,12 @@
         <f t="shared" si="0"/>
         <v>4605.5164992718474</v>
       </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>116.61649927184772</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -11038,6 +11344,10 @@
       <c r="D10">
         <f t="shared" si="0"/>
         <v>6054.760911587291</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>178.06091158729123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>